<commit_message>
Pushing the stack implementations
</commit_message>
<xml_diff>
--- a/Dynamic Programing/Dynamic Programing Geeks.xlsx
+++ b/Dynamic Programing/Dynamic Programing Geeks.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IIIT B SEM 1\Algorithms\Dynamic Programing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Data-Structure-and-Algorithms\Dynamic Programing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="187">
   <si>
     <t>Basic Problems :</t>
   </si>
@@ -939,8 +939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C187"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,82 +1070,109 @@
         <v>186</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
@@ -1316,7 +1343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView topLeftCell="A114" workbookViewId="0">
+    <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="B136" sqref="B136"/>
     </sheetView>
   </sheetViews>

</xml_diff>